<commit_message>
Added test cases and cleaned up code
</commit_message>
<xml_diff>
--- a/testdata/processed/carsXlsx.xlsx
+++ b/testdata/processed/carsXlsx.xlsx
@@ -397,7 +397,7 @@
       <c r="A2" t="str">
         <v>Audi</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
         <v>10000</v>
       </c>
       <c r="C2" t="str">
@@ -419,7 +419,7 @@
       <c r="A4" t="str">
         <v>Mercedes</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
         <v>20000</v>
       </c>
       <c r="C4" t="str">

</xml_diff>